<commit_message>
Adição da função de adicionar linhas caso o documento já exista
</commit_message>
<xml_diff>
--- a/Reclame Aqui.xlsx
+++ b/Reclame Aqui.xlsx
@@ -175,10 +175,10 @@
     <t>Geral</t>
   </si>
   <si>
-    <t>15/05/2021</t>
-  </si>
-  <si>
-    <t>14/05/2024</t>
+    <t>16/05/2021</t>
+  </si>
+  <si>
+    <t>15/05/2024</t>
   </si>
   <si>
     <t>7.1</t>

</xml_diff>